<commit_message>
Model runs and updated plots
</commit_message>
<xml_diff>
--- a/results/Manuscript/total_capacity.xlsx
+++ b/results/Manuscript/total_capacity.xlsx
@@ -111,7 +111,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="67">
+  <fills count="113">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -126,19 +126,205 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFACACF6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF4C4CFB"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0B0BFE"/>
+        <fgColor rgb="FFB9B9F6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8686F8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6B6BFA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFABABF6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5959FA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0D0DFE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFADADF6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5B5BFA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF1010FE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB5B5F6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7F7FF9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6464FA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA8A8F6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5555FB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0A0AFE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAAAAF6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5757FB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0C0CFE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAEAEF6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7676F9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA6A6F7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4B4BFB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0606FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA7A7F7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4D4DFB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB2B2F6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6F6FF9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5252FB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4646FB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0404FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4949FB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0505FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6767FA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4F4FFB"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -150,25 +336,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF3E3EFC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0101FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA4A4F7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF3D3DFC"/>
+        <fgColor rgb="FF4343FC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0202FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0303FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA9A9F6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5E5EFA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3F3FFC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -180,79 +378,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFAAAAF6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF4A4AFB"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0909FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA7A7F7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF4545FB"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0505FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF4949FB"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0808FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA8A8F6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF4747FB"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0707FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF4343FC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0303FF"/>
+        <fgColor rgb="FF4040FC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -282,31 +408,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFE7F1E7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE3EFE3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD3E7D3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE9F2E9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE8F2E8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9FCE9F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF69B369"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF349A34"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDEEDDE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCAE3CA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF94C994"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE0EEDF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE6F1E6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB9DBB9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF91C791"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6EB66E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE1EEE1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBBDCBB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFEAF2EA"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF9FCE9F"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF69B369"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF349A34"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE8F2E8"/>
+        <fgColor rgb="FF9BCC9B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4BA54A"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF008000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCE4CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF96C996"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -318,55 +558,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFB9DBB9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF91C791"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF6EB66E"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF9BCC9B"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF4BA54A"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF008000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE9F2E9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE6F1E6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE7F1E7"/>
+        <fgColor rgb="FFE4F0E4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -390,19 +582,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF4EADB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6DBAA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8D18A"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF3EEE8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF4ECE0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF3EDE4"/>
+        <fgColor rgb="FFF4E8D3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4EBDF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3EEE7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4E7D1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4EBDD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF7D69A"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF9CA76"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3ECE2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6DFB7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6DBAB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3EFEC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3EDE5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3EFEB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4E9D8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3EDE3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3F0ED"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5E3C3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5E1BE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -414,49 +720,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF3F0ED"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF4E8D3"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF7D69A"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF9CA76"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF3EFEC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF3EEE7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF5E3C3"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF5E1BE"/>
+        <fgColor rgb="FFF4E8D4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -468,7 +732,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF3EDE6"/>
+        <fgColor rgb="FFF4ECE1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5E1BF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF7D79E"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -480,13 +756,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF6DBAA"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF7D597"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4E6CF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -536,7 +812,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -544,8 +820,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -553,39 +829,39 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="48" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -606,7 +882,53 @@
     <xf numFmtId="0" fontId="2" fillId="63" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="64" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="65" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="66" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="66" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="67" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="68" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="69" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="70" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="71" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="72" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="73" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="74" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="75" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="76" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="77" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="78" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="79" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="80" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="81" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="82" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="83" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="84" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="85" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="86" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="87" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="88" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="89" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="90" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="91" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="92" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="93" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="94" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="95" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="96" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="97" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="98" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="99" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="100" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="101" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="102" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="103" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="104" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="105" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="106" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="107" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="108" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="109" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="110" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="111" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="112" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1001,7 +1323,7 @@
         <v>11</v>
       </c>
       <c r="F5" s="4">
-        <v>565.9152544174246</v>
+        <v>483.12078453503</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1021,7 +1343,7 @@
         <v>14</v>
       </c>
       <c r="F6" s="5">
-        <v>1340.179112074856</v>
+        <v>923.1831725841055</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1041,7 +1363,7 @@
         <v>15</v>
       </c>
       <c r="F7" s="6">
-        <v>1871.669320701552</v>
+        <v>1152.751003947368</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1061,7 +1383,7 @@
         <v>11</v>
       </c>
       <c r="F8" s="7">
-        <v>620.7502161710411</v>
+        <v>605.8979066706646</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1081,7 +1403,7 @@
         <v>14</v>
       </c>
       <c r="F9" s="8">
-        <v>1454.94711491725</v>
+        <v>1317.249133481703</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1101,7 +1423,7 @@
         <v>15</v>
       </c>
       <c r="F10" s="9">
-        <v>1956.327374914845</v>
+        <v>1965.52415509424</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1121,7 +1443,7 @@
         <v>11</v>
       </c>
       <c r="F11" s="10">
-        <v>623.342815174823</v>
+        <v>594.3782323951318</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1141,7 +1463,7 @@
         <v>14</v>
       </c>
       <c r="F12" s="11">
-        <v>1462.713331941743</v>
+        <v>1301.879148750203</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1161,7 +1483,7 @@
         <v>15</v>
       </c>
       <c r="F13" s="12">
-        <v>1966.766116343693</v>
+        <v>1943.557311694308</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1241,7 +1563,7 @@
         <v>11</v>
       </c>
       <c r="F17" s="13">
-        <v>582.8185979174182</v>
+        <v>516.7393436324022</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1261,7 +1583,7 @@
         <v>14</v>
       </c>
       <c r="F18" s="14">
-        <v>1357.08245557485</v>
+        <v>977.8659786286419</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1281,7 +1603,7 @@
         <v>15</v>
       </c>
       <c r="F19" s="15">
-        <v>1888.572664201545</v>
+        <v>1216.650628157832</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1300,8 +1622,8 @@
       <c r="E20" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F20" s="7">
-        <v>622.0334160007335</v>
+      <c r="F20" s="16">
+        <v>627.2015891316861</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1320,8 +1642,8 @@
       <c r="E21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F21" s="8">
-        <v>1457.93975091872</v>
+      <c r="F21" s="17">
+        <v>1350.567597398343</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1340,8 +1662,8 @@
       <c r="E22" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F22" s="12">
-        <v>1959.434869202987</v>
+      <c r="F22" s="18">
+        <v>1993.216796156673</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1360,8 +1682,8 @@
       <c r="E23" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="10">
-        <v>623.342815174823</v>
+      <c r="F23" s="19">
+        <v>615.9845044264446</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1380,8 +1702,8 @@
       <c r="E24" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F24" s="11">
-        <v>1462.713331941743</v>
+      <c r="F24" s="20">
+        <v>1331.708582166876</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1400,8 +1722,8 @@
       <c r="E25" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F25" s="12">
-        <v>1966.822099623048</v>
+      <c r="F25" s="21">
+        <v>1975.277432470191</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1480,8 +1802,8 @@
       <c r="E29" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="16">
-        <v>601.7840211400251</v>
+      <c r="F29" s="22">
+        <v>570.2340431172195</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1500,8 +1822,8 @@
       <c r="E30" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F30" s="17">
-        <v>1398.910292793575</v>
+      <c r="F30" s="23">
+        <v>1062.9119307393</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1520,8 +1842,8 @@
       <c r="E31" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F31" s="18">
-        <v>1926.484276448094</v>
+      <c r="F31" s="15">
+        <v>1216.650628157832</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1540,8 +1862,8 @@
       <c r="E32" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F32" s="7">
-        <v>622.25114723056</v>
+      <c r="F32" s="24">
+        <v>644.9321684842531</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1560,8 +1882,8 @@
       <c r="E33" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F33" s="8">
-        <v>1459.280047838208</v>
+      <c r="F33" s="25">
+        <v>1426.160769060212</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1580,8 +1902,8 @@
       <c r="E34" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F34" s="12">
-        <v>1962.033476701951</v>
+      <c r="F34" s="26">
+        <v>2027.849145965239</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1600,8 +1922,8 @@
       <c r="E35" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F35" s="10">
-        <v>623.342815174823</v>
+      <c r="F35" s="27">
+        <v>639.4866324486115</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1620,8 +1942,8 @@
       <c r="E36" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F36" s="11">
-        <v>1462.713331941743</v>
+      <c r="F36" s="28">
+        <v>1409.052977442889</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1640,8 +1962,8 @@
       <c r="E37" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F37" s="12">
-        <v>1967.048943448735</v>
+      <c r="F37" s="26">
+        <v>2029.720920787313</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1720,8 +2042,8 @@
       <c r="E41" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F41" s="13">
-        <v>578.9143574202435</v>
+      <c r="F41" s="29">
+        <v>544.1390201710497</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1740,8 +2062,8 @@
       <c r="E42" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F42" s="19">
-        <v>1369.913837685192</v>
+      <c r="F42" s="30">
+        <v>1117.765513126117</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1760,8 +2082,8 @@
       <c r="E43" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F43" s="20">
-        <v>1893.838803655416</v>
+      <c r="F43" s="31">
+        <v>1369.900126978853</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1780,8 +2102,8 @@
       <c r="E44" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F44" s="7">
-        <v>621.7878866530157</v>
+      <c r="F44" s="27">
+        <v>641.1266007144516</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1800,8 +2122,8 @@
       <c r="E45" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F45" s="8">
-        <v>1458.448850249273</v>
+      <c r="F45" s="32">
+        <v>1480.185886249178</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1820,8 +2142,8 @@
       <c r="E46" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F46" s="12">
-        <v>1960.017561280078</v>
+      <c r="F46" s="33">
+        <v>2049.674743127431</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1840,8 +2162,8 @@
       <c r="E47" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F47" s="10">
-        <v>623.342815174823</v>
+      <c r="F47" s="27">
+        <v>637.9581645781425</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1860,8 +2182,8 @@
       <c r="E48" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F48" s="11">
-        <v>1462.713331941743</v>
+      <c r="F48" s="34">
+        <v>1452.185526283143</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1880,8 +2202,8 @@
       <c r="E49" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F49" s="12">
-        <v>1966.91506012143</v>
+      <c r="F49" s="35">
+        <v>2037.810921743861</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1960,8 +2282,8 @@
       <c r="E53" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F53" s="21">
-        <v>592.3301912343321</v>
+      <c r="F53" s="10">
+        <v>578.6995966935914</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1980,8 +2302,8 @@
       <c r="E54" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F54" s="22">
-        <v>1387.405160866716</v>
+      <c r="F54" s="36">
+        <v>1193.718513582891</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -2000,8 +2322,8 @@
       <c r="E55" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F55" s="23">
-        <v>1907.254637469505</v>
+      <c r="F55" s="37">
+        <v>1394.001501279783</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -2020,8 +2342,8 @@
       <c r="E56" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F56" s="7">
-        <v>622.3829108389771</v>
+      <c r="F56" s="38">
+        <v>653.4724117453472</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -2040,8 +2362,8 @@
       <c r="E57" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F57" s="8">
-        <v>1459.619904785944</v>
+      <c r="F57" s="39">
+        <v>1499.453134140224</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -2060,8 +2382,8 @@
       <c r="E58" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F58" s="12">
-        <v>1961.47739950612</v>
+      <c r="F58" s="40">
+        <v>2064.334238553281</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -2080,8 +2402,8 @@
       <c r="E59" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F59" s="10">
-        <v>623.342815174823</v>
+      <c r="F59" s="38">
+        <v>651.7108701284687</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -2100,8 +2422,8 @@
       <c r="E60" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F60" s="11">
-        <v>1462.713331941743</v>
+      <c r="F60" s="32">
+        <v>1478.927633176474</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -2120,8 +2442,8 @@
       <c r="E61" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F61" s="12">
-        <v>1966.949756649185</v>
+      <c r="F61" s="41">
+        <v>2057.710104037031</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -2200,8 +2522,8 @@
       <c r="E65" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F65" s="16">
-        <v>606.6869826922898</v>
+      <c r="F65" s="42">
+        <v>619.8700563430664</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -2220,8 +2542,8 @@
       <c r="E66" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F66" s="24">
-        <v>1419.727868000706</v>
+      <c r="F66" s="43">
+        <v>1263.869862652072</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -2240,8 +2562,8 @@
       <c r="E67" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F67" s="25">
-        <v>1938.101392957686</v>
+      <c r="F67" s="37">
+        <v>1394.001501279783</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -2260,8 +2582,8 @@
       <c r="E68" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F68" s="10">
-        <v>622.634057984588</v>
+      <c r="F68" s="38">
+        <v>659.0796714290118</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -2280,8 +2602,8 @@
       <c r="E69" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F69" s="11">
-        <v>1460.692678108664</v>
+      <c r="F69" s="44">
+        <v>1534.149384223912</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -2300,8 +2622,8 @@
       <c r="E70" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F70" s="12">
-        <v>1963.397805041242</v>
+      <c r="F70" s="45">
+        <v>2084.522286770332</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -2320,8 +2642,8 @@
       <c r="E71" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F71" s="10">
-        <v>623.342815174823</v>
+      <c r="F71" s="38">
+        <v>657.2982506168862</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -2340,8 +2662,8 @@
       <c r="E72" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F72" s="11">
-        <v>1462.713331941743</v>
+      <c r="F72" s="46">
+        <v>1524.821920266571</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -2360,8 +2682,8 @@
       <c r="E73" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F73" s="12">
-        <v>1967.08223898001</v>
+      <c r="F73" s="45">
+        <v>2080.323524544172</v>
       </c>
     </row>
   </sheetData>
@@ -2410,7 +2732,7 @@
       <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="26">
+      <c r="F2" s="47">
         <v>0</v>
       </c>
     </row>
@@ -2430,7 +2752,7 @@
       <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="26">
+      <c r="F3" s="47">
         <v>0</v>
       </c>
     </row>
@@ -2450,7 +2772,7 @@
       <c r="E4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="26">
+      <c r="F4" s="47">
         <v>0</v>
       </c>
     </row>
@@ -2470,7 +2792,7 @@
       <c r="E5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="26">
+      <c r="F5" s="47">
         <v>0</v>
       </c>
     </row>
@@ -2490,7 +2812,7 @@
       <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="26">
+      <c r="F6" s="47">
         <v>0</v>
       </c>
     </row>
@@ -2510,7 +2832,7 @@
       <c r="E7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="26">
+      <c r="F7" s="47">
         <v>0</v>
       </c>
     </row>
@@ -2530,7 +2852,7 @@
       <c r="E8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="26">
+      <c r="F8" s="47">
         <v>0</v>
       </c>
     </row>
@@ -2550,7 +2872,7 @@
       <c r="E9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="26">
+      <c r="F9" s="47">
         <v>0</v>
       </c>
     </row>
@@ -2570,7 +2892,7 @@
       <c r="E10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="26">
+      <c r="F10" s="47">
         <v>0</v>
       </c>
     </row>
@@ -2590,7 +2912,7 @@
       <c r="E11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="26">
+      <c r="F11" s="47">
         <v>0</v>
       </c>
     </row>
@@ -2610,7 +2932,7 @@
       <c r="E12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="26">
+      <c r="F12" s="47">
         <v>0</v>
       </c>
     </row>
@@ -2630,7 +2952,7 @@
       <c r="E13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="26">
+      <c r="F13" s="47">
         <v>0</v>
       </c>
     </row>
@@ -2650,8 +2972,8 @@
       <c r="E14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="27">
-        <v>616.2619429148438</v>
+      <c r="F14" s="48">
+        <v>616.2619429148439</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2670,8 +2992,8 @@
       <c r="E15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="28">
-        <v>1075.808909626444</v>
+      <c r="F15" s="49">
+        <v>1075.808909626445</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2690,8 +3012,8 @@
       <c r="E16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="29">
-        <v>1319.070738412528</v>
+      <c r="F16" s="50">
+        <v>1319.070738412529</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2710,8 +3032,8 @@
       <c r="E17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="30">
-        <v>24.7366827661403</v>
+      <c r="F17" s="51">
+        <v>68.62344430462659</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2730,8 +3052,8 @@
       <c r="E18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="30">
-        <v>24.7366827661403</v>
+      <c r="F18" s="52">
+        <v>123.382203195936</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2750,8 +3072,8 @@
       <c r="E19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="30">
-        <v>24.7366827661403</v>
+      <c r="F19" s="53">
+        <v>364.4666266399108</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2770,8 +3092,8 @@
       <c r="E20" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F20" s="26">
-        <v>1.721201479431673</v>
+      <c r="F20" s="54">
+        <v>31.4492424985207</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2790,8 +3112,8 @@
       <c r="E21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F21" s="26">
-        <v>3.990945371962852</v>
+      <c r="F21" s="51">
+        <v>60.37855996830722</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -2810,8 +3132,8 @@
       <c r="E22" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F22" s="26">
-        <v>4.129341951426044</v>
+      <c r="F22" s="55">
+        <v>53.87988420038165</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -2830,8 +3152,8 @@
       <c r="E23" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="26">
-        <v>0</v>
+      <c r="F23" s="54">
+        <v>33.12524638344903</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -2850,8 +3172,8 @@
       <c r="E24" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F24" s="26">
-        <v>0</v>
+      <c r="F24" s="55">
+        <v>53.49084226871565</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -2870,8 +3192,8 @@
       <c r="E25" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F25" s="26">
-        <v>0.06194088324613722</v>
+      <c r="F25" s="55">
+        <v>50.99647979473985</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -2890,7 +3212,7 @@
       <c r="E26" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F26" s="31">
+      <c r="F26" s="56">
         <v>1147.271624831435</v>
       </c>
     </row>
@@ -2910,7 +3232,7 @@
       <c r="E27" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F27" s="32">
+      <c r="F27" s="57">
         <v>1953.1432449587</v>
       </c>
     </row>
@@ -2930,7 +3252,7 @@
       <c r="E28" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F28" s="33">
+      <c r="F28" s="58">
         <v>2738.730225682273</v>
       </c>
     </row>
@@ -2950,8 +3272,8 @@
       <c r="E29" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="34">
-        <v>52.66512742172172</v>
+      <c r="F29" s="59">
+        <v>203.1680193021543</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -2970,8 +3292,8 @@
       <c r="E30" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F30" s="35">
-        <v>85.70618179403229</v>
+      <c r="F30" s="60">
+        <v>495.1232989097524</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -2990,8 +3312,8 @@
       <c r="E31" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F31" s="35">
-        <v>84.01864744187954</v>
+      <c r="F31" s="61">
+        <v>1306.653953097716</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -3010,8 +3332,8 @@
       <c r="E32" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F32" s="26">
-        <v>2.256665676135701</v>
+      <c r="F32" s="51">
+        <v>58.28292627013489</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -3030,8 +3352,8 @@
       <c r="E33" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F33" s="26">
-        <v>6.433353256355201</v>
+      <c r="F33" s="59">
+        <v>204.8798529795227</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -3050,8 +3372,8 @@
       <c r="E34" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F34" s="26">
-        <v>8.57916095491996</v>
+      <c r="F34" s="62">
+        <v>173.1823420834153</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -3070,8 +3392,8 @@
       <c r="E35" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F35" s="26">
-        <v>0</v>
+      <c r="F35" s="63">
+        <v>70.56254658121432</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -3090,8 +3412,8 @@
       <c r="E36" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F36" s="26">
-        <v>0</v>
+      <c r="F36" s="59">
+        <v>199.8002246283588</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -3110,8 +3432,8 @@
       <c r="E37" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F37" s="26">
-        <v>0.3210427361123303</v>
+      <c r="F37" s="62">
+        <v>168.6425823170192</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -3130,7 +3452,7 @@
       <c r="E38" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F38" s="26">
+      <c r="F38" s="47">
         <v>0</v>
       </c>
     </row>
@@ -3150,7 +3472,7 @@
       <c r="E39" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F39" s="26">
+      <c r="F39" s="47">
         <v>0</v>
       </c>
     </row>
@@ -3170,7 +3492,7 @@
       <c r="E40" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F40" s="26">
+      <c r="F40" s="47">
         <v>0</v>
       </c>
     </row>
@@ -3190,7 +3512,7 @@
       <c r="E41" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F41" s="26">
+      <c r="F41" s="47">
         <v>0</v>
       </c>
     </row>
@@ -3210,7 +3532,7 @@
       <c r="E42" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F42" s="26">
+      <c r="F42" s="47">
         <v>0</v>
       </c>
     </row>
@@ -3230,7 +3552,7 @@
       <c r="E43" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F43" s="26">
+      <c r="F43" s="47">
         <v>0</v>
       </c>
     </row>
@@ -3250,7 +3572,7 @@
       <c r="E44" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F44" s="26">
+      <c r="F44" s="47">
         <v>0</v>
       </c>
     </row>
@@ -3270,7 +3592,7 @@
       <c r="E45" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F45" s="26">
+      <c r="F45" s="47">
         <v>0</v>
       </c>
     </row>
@@ -3290,7 +3612,7 @@
       <c r="E46" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F46" s="26">
+      <c r="F46" s="47">
         <v>0</v>
       </c>
     </row>
@@ -3310,7 +3632,7 @@
       <c r="E47" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F47" s="26">
+      <c r="F47" s="47">
         <v>0</v>
       </c>
     </row>
@@ -3330,7 +3652,7 @@
       <c r="E48" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F48" s="26">
+      <c r="F48" s="47">
         <v>0</v>
       </c>
     </row>
@@ -3350,7 +3672,7 @@
       <c r="E49" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F49" s="26">
+      <c r="F49" s="47">
         <v>0</v>
       </c>
     </row>
@@ -3370,8 +3692,8 @@
       <c r="E50" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F50" s="36">
-        <v>759.2297272366442</v>
+      <c r="F50" s="64">
+        <v>759.2297272366443</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -3390,7 +3712,7 @@
       <c r="E51" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F51" s="37">
+      <c r="F51" s="65">
         <v>1354.448307248184</v>
       </c>
     </row>
@@ -3410,7 +3732,7 @@
       <c r="E52" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F52" s="38">
+      <c r="F52" s="66">
         <v>1873.781221153102</v>
       </c>
     </row>
@@ -3430,8 +3752,8 @@
       <c r="E53" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F53" s="30">
-        <v>17.9039684322433</v>
+      <c r="F53" s="55">
+        <v>47.97742029878688</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -3450,8 +3772,8 @@
       <c r="E54" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F54" s="30">
-        <v>24.71348940620958</v>
+      <c r="F54" s="67">
+        <v>139.3228605696621</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -3470,8 +3792,8 @@
       <c r="E55" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F55" s="30">
-        <v>17.9039684322433</v>
+      <c r="F55" s="68">
+        <v>726.9746725108813</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -3490,8 +3812,8 @@
       <c r="E56" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F56" s="26">
-        <v>0.7630664063589053</v>
+      <c r="F56" s="69">
+        <v>16.08545935837178</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -3510,8 +3832,8 @@
       <c r="E57" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F57" s="26">
-        <v>1.532187398651487</v>
+      <c r="F57" s="54">
+        <v>27.72313477612434</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -3530,8 +3852,8 @@
       <c r="E58" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F58" s="26">
-        <v>1.884584859553688</v>
+      <c r="F58" s="69">
+        <v>20.24594606881279</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -3550,8 +3872,8 @@
       <c r="E59" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F59" s="26">
-        <v>0</v>
+      <c r="F59" s="69">
+        <v>19.23173885121909</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -3570,8 +3892,8 @@
       <c r="E60" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F60" s="26">
-        <v>0</v>
+      <c r="F60" s="54">
+        <v>35.0814098334927</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -3590,8 +3912,8 @@
       <c r="E61" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F61" s="26">
-        <v>0.03838884751747525</v>
+      <c r="F61" s="69">
+        <v>25.29289472196106</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -3610,7 +3932,7 @@
       <c r="E62" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F62" s="39">
+      <c r="F62" s="70">
         <v>1197.134754443719</v>
       </c>
     </row>
@@ -3630,7 +3952,7 @@
       <c r="E63" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F63" s="40">
+      <c r="F63" s="71">
         <v>2417.958950560746</v>
       </c>
     </row>
@@ -3650,7 +3972,7 @@
       <c r="E64" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F64" s="41">
+      <c r="F64" s="72">
         <v>3538.613576294043</v>
       </c>
     </row>
@@ -3670,8 +3992,8 @@
       <c r="E65" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F65" s="42">
-        <v>38.86259409460152</v>
+      <c r="F65" s="52">
+        <v>114.5834803005756</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -3690,8 +4012,8 @@
       <c r="E66" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F66" s="43">
-        <v>75.81956380984481</v>
+      <c r="F66" s="73">
+        <v>457.5275225094762</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -3710,8 +4032,8 @@
       <c r="E67" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F67" s="44">
-        <v>63.84598799011226</v>
+      <c r="F67" s="74">
+        <v>1276.88334455429</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -3730,8 +4052,8 @@
       <c r="E68" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F68" s="26">
-        <v>1.195403724221273</v>
+      <c r="F68" s="69">
+        <v>25.55812244389284</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -3750,8 +4072,8 @@
       <c r="E69" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F69" s="26">
-        <v>3.247314346877608</v>
+      <c r="F69" s="75">
+        <v>85.04682687406506</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -3770,8 +4092,8 @@
       <c r="E70" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F70" s="26">
-        <v>4.756952720689417</v>
+      <c r="F70" s="51">
+        <v>55.87992085895756</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -3790,8 +4112,8 @@
       <c r="E71" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F71" s="26">
-        <v>0</v>
+      <c r="F71" s="54">
+        <v>29.69897916076388</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -3810,8 +4132,8 @@
       <c r="E72" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F72" s="26">
-        <v>0</v>
+      <c r="F72" s="76">
+        <v>106.2937780279886</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -3830,8 +4152,8 @@
       <c r="E73" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F73" s="26">
-        <v>0.1897106535437932</v>
+      <c r="F73" s="51">
+        <v>65.99310399251166</v>
       </c>
     </row>
   </sheetData>
@@ -3880,7 +4202,7 @@
       <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="45">
+      <c r="F2" s="77">
         <v>515.7983333314282</v>
       </c>
     </row>
@@ -3900,7 +4222,7 @@
       <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="46">
+      <c r="F3" s="78">
         <v>1203.150497316135</v>
       </c>
     </row>
@@ -3920,7 +4242,7 @@
       <c r="E4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="47">
+      <c r="F4" s="79">
         <v>1592.544718744919</v>
       </c>
     </row>
@@ -3940,8 +4262,8 @@
       <c r="E5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="48">
-        <v>44.26054413735847</v>
+      <c r="F5" s="80">
+        <v>134.3053731443071</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -3960,8 +4282,8 @@
       <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="49">
-        <v>95.01390293371325</v>
+      <c r="F6" s="81">
+        <v>454.3618084992925</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -3980,8 +4302,8 @@
       <c r="E7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="50">
-        <v>73.73698404959765</v>
+      <c r="F7" s="82">
+        <v>667.3249808243377</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -4000,8 +4322,8 @@
       <c r="E8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="51">
-        <v>1.936352364409015</v>
+      <c r="F8" s="83">
+        <v>46.38043355645637</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -4020,8 +4342,8 @@
       <c r="E9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="51">
-        <v>5.761525304311214</v>
+      <c r="F9" s="84">
+        <v>182.4978379949073</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -4040,8 +4362,8 @@
       <c r="E10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="52">
-        <v>8.228526999026389</v>
+      <c r="F10" s="85">
+        <v>104.1655418559661</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -4060,8 +4382,8 @@
       <c r="E11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="51">
-        <v>0</v>
+      <c r="F11" s="86">
+        <v>54.78436092290551</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -4080,8 +4402,8 @@
       <c r="E12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="51">
-        <v>0</v>
+      <c r="F12" s="87">
+        <v>194.1929445856546</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -4100,8 +4422,8 @@
       <c r="E13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="51">
-        <v>0.474532612948954</v>
+      <c r="F13" s="88">
+        <v>120.411246992468</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -4120,7 +4442,7 @@
       <c r="E14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="53">
+      <c r="F14" s="84">
         <v>183.7625431282737</v>
       </c>
     </row>
@@ -4140,7 +4462,7 @@
       <c r="E15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="54">
+      <c r="F15" s="89">
         <v>564.8558930484317</v>
       </c>
     </row>
@@ -4160,7 +4482,7 @@
       <c r="E16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="55">
+      <c r="F16" s="90">
         <v>803.5661598844738</v>
       </c>
     </row>
@@ -4180,8 +4502,8 @@
       <c r="E17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="56">
-        <v>22.70962231469279</v>
+      <c r="F17" s="91">
+        <v>84.82386276273837</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -4200,8 +4522,8 @@
       <c r="E18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="50">
-        <v>73.46298111104755</v>
+      <c r="F18" s="92">
+        <v>367.4292698011744</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -4220,8 +4542,8 @@
       <c r="E19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="57">
-        <v>52.18606222693199</v>
+      <c r="F19" s="93">
+        <v>452.9940195118803</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -4240,8 +4562,8 @@
       <c r="E20" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F20" s="51">
-        <v>0.3021161210002949</v>
+      <c r="F20" s="94">
+        <v>20.28153675045895</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -4260,8 +4582,8 @@
       <c r="E21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F21" s="51">
-        <v>1.967559390991002</v>
+      <c r="F21" s="80">
+        <v>136.8393397935809</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -4280,8 +4602,8 @@
       <c r="E22" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F22" s="51">
-        <v>4.296164506242987</v>
+      <c r="F22" s="95">
+        <v>65.0308742471066</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -4300,8 +4622,8 @@
       <c r="E23" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="51">
-        <v>0</v>
+      <c r="F23" s="96">
+        <v>27.71744338716682</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -4320,8 +4642,8 @@
       <c r="E24" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F24" s="51">
-        <v>0</v>
+      <c r="F24" s="97">
+        <v>153.4042032650071</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -4340,8 +4662,8 @@
       <c r="E25" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F25" s="51">
-        <v>0.4088092642435778</v>
+      <c r="F25" s="98">
+        <v>79.62250567182066</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -4360,7 +4682,7 @@
       <c r="E26" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F26" s="52">
+      <c r="F26" s="99">
         <v>17.03713432198739</v>
       </c>
     </row>
@@ -4380,8 +4702,8 @@
       <c r="E27" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F27" s="58">
-        <v>287.2318664885298</v>
+      <c r="F27" s="100">
+        <v>287.2318664885297</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -4400,8 +4722,8 @@
       <c r="E28" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F28" s="59">
-        <v>328.3449640089807</v>
+      <c r="F28" s="101">
+        <v>328.3449640089808</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -4420,8 +4742,8 @@
       <c r="E29" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="51">
-        <v>0</v>
+      <c r="F29" s="102">
+        <v>2.324118779117084</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -4440,8 +4762,8 @@
       <c r="E30" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F30" s="56">
-        <v>22.59732434760382</v>
+      <c r="F30" s="103">
+        <v>176.0546189652882</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -4460,8 +4782,8 @@
       <c r="E31" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F31" s="51">
-        <v>4.844419821488441</v>
+      <c r="F31" s="80">
+        <v>134.8578475370718</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -4480,7 +4802,7 @@
       <c r="E32" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F32" s="51">
+      <c r="F32" s="102">
         <v>0</v>
       </c>
     </row>
@@ -4500,8 +4822,8 @@
       <c r="E33" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F33" s="51">
-        <v>0.2051261322193287</v>
+      <c r="F33" s="104">
+        <v>36.96416854849968</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -4520,8 +4842,8 @@
       <c r="E34" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F34" s="51">
-        <v>0.8695242873460773</v>
+      <c r="F34" s="102">
+        <v>0.8768219189023396</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -4540,7 +4862,7 @@
       <c r="E35" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F35" s="51">
+      <c r="F35" s="102">
         <v>0</v>
       </c>
     </row>
@@ -4560,8 +4882,8 @@
       <c r="E36" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F36" s="51">
-        <v>0</v>
+      <c r="F36" s="86">
+        <v>51.42141036601843</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -4580,8 +4902,8 @@
       <c r="E37" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F37" s="51">
-        <v>0.1500571724585605</v>
+      <c r="F37" s="102">
+        <v>3.462995388394147</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -4600,7 +4922,7 @@
       <c r="E38" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F38" s="45">
+      <c r="F38" s="77">
         <v>515.7983333314282</v>
       </c>
     </row>
@@ -4620,7 +4942,7 @@
       <c r="E39" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F39" s="46">
+      <c r="F39" s="78">
         <v>1203.150497316135</v>
       </c>
     </row>
@@ -4640,7 +4962,7 @@
       <c r="E40" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F40" s="47">
+      <c r="F40" s="79">
         <v>1592.544718744919</v>
       </c>
     </row>
@@ -4660,8 +4982,8 @@
       <c r="E41" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F41" s="60">
-        <v>33.92157739486524</v>
+      <c r="F41" s="105">
+        <v>91.05292679505567</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -4680,8 +5002,8 @@
       <c r="E42" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F42" s="50">
-        <v>71.2750733561096</v>
+      <c r="F42" s="106">
+        <v>321.5262058651348</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -4700,8 +5022,8 @@
       <c r="E43" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F43" s="61">
-        <v>56.05545046388953</v>
+      <c r="F43" s="107">
+        <v>536.1615916173696</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -4720,8 +5042,8 @@
       <c r="E44" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F44" s="51">
-        <v>1.172271354296421</v>
+      <c r="F44" s="94">
+        <v>21.14379388521164</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -4740,8 +5062,8 @@
       <c r="E45" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F45" s="51">
-        <v>3.189691974707481</v>
+      <c r="F45" s="95">
+        <v>65.82631989830935</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -4760,8 +5082,8 @@
       <c r="E46" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F46" s="51">
-        <v>5.518297089959466</v>
+      <c r="F46" s="83">
+        <v>44.18782887180122</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -4780,8 +5102,8 @@
       <c r="E47" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F47" s="51">
-        <v>0</v>
+      <c r="F47" s="94">
+        <v>23.44644400454487</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -4800,8 +5122,8 @@
       <c r="E48" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F48" s="51">
-        <v>0</v>
+      <c r="F48" s="91">
+        <v>86.24062205008727</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -4820,8 +5142,8 @@
       <c r="E49" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F49" s="51">
-        <v>0.3599318234696518</v>
+      <c r="F49" s="86">
+        <v>52.81883861675564</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -4840,8 +5162,8 @@
       <c r="E50" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F50" s="62">
-        <v>130.5635813865584</v>
+      <c r="F50" s="108">
+        <v>130.5635813865583</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -4860,7 +5182,7 @@
       <c r="E51" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F51" s="63">
+      <c r="F51" s="81">
         <v>459.4908617846568</v>
       </c>
     </row>
@@ -4880,8 +5202,8 @@
       <c r="E52" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F52" s="64">
-        <v>583.2422931874853</v>
+      <c r="F52" s="109">
+        <v>583.2422931874851</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -4900,8 +5222,8 @@
       <c r="E53" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F53" s="52">
-        <v>17.37834277799846</v>
+      <c r="F53" s="83">
+        <v>49.56131869794132</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -4920,8 +5242,8 @@
       <c r="E54" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F54" s="48">
-        <v>49.35413348428072</v>
+      <c r="F54" s="110">
+        <v>213.6944929801791</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -4940,8 +5262,8 @@
       <c r="E55" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F55" s="65">
-        <v>39.51221584702273</v>
+      <c r="F55" s="103">
+        <v>178.0814745941907</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -4960,8 +5282,8 @@
       <c r="E56" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F56" s="51">
-        <v>0.4273792104589046</v>
+      <c r="F56" s="99">
+        <v>6.756301976429436</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -4980,8 +5302,8 @@
       <c r="E57" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F57" s="51">
-        <v>1.710847809862805</v>
+      <c r="F57" s="111">
+        <v>42.51319236584933</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -5000,8 +5322,8 @@
       <c r="E58" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F58" s="51">
-        <v>3.68705546421259</v>
+      <c r="F58" s="96">
+        <v>26.73443233736913</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -5020,8 +5342,8 @@
       <c r="E59" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F59" s="51">
-        <v>0</v>
+      <c r="F59" s="99">
+        <v>6.903209387678077</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -5040,8 +5362,8 @@
       <c r="E60" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F60" s="51">
-        <v>0</v>
+      <c r="F60" s="86">
+        <v>54.97147660664991</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -5060,8 +5382,8 @@
       <c r="E61" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F61" s="51">
-        <v>0.319198732826391</v>
+      <c r="F61" s="96">
+        <v>29.86728322668818</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -5080,7 +5402,7 @@
       <c r="E62" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F62" s="51">
+      <c r="F62" s="102">
         <v>0.1178186833649647</v>
       </c>
     </row>
@@ -5100,7 +5422,7 @@
       <c r="E63" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F63" s="62">
+      <c r="F63" s="108">
         <v>127.5892090831109</v>
       </c>
     </row>
@@ -5120,8 +5442,8 @@
       <c r="E64" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F64" s="57">
-        <v>51.35203405575294</v>
+      <c r="F64" s="86">
+        <v>51.35203405575305</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -5140,8 +5462,8 @@
       <c r="E65" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F65" s="51">
-        <v>0.1178177020944756</v>
+      <c r="F65" s="102">
+        <v>0.1178186519249901</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -5160,8 +5482,8 @@
       <c r="E66" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F66" s="52">
-        <v>8.892161596421589</v>
+      <c r="F66" s="86">
+        <v>52.2063639349315</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -5180,8 +5502,8 @@
       <c r="E67" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F67" s="51">
-        <v>1.490532331558613</v>
+      <c r="F67" s="99">
+        <v>8.545459160627047</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -5200,8 +5522,8 @@
       <c r="E68" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F68" s="51">
-        <v>0.1090910646711687</v>
+      <c r="F68" s="102">
+        <v>0.1175390498553906</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -5220,8 +5542,8 @@
       <c r="E69" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F69" s="51">
-        <v>0.3365625140071203</v>
+      <c r="F69" s="102">
+        <v>0.3450104991913423</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -5240,8 +5562,8 @@
       <c r="E70" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F70" s="51">
-        <v>1.267902199329418</v>
+      <c r="F70" s="102">
+        <v>1.449974475261339</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -5260,8 +5582,8 @@
       <c r="E71" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F71" s="51">
-        <v>0</v>
+      <c r="F71" s="102">
+        <v>0.09085353363962542</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -5280,8 +5602,8 @@
       <c r="E72" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F72" s="51">
-        <v>0</v>
+      <c r="F72" s="102">
+        <v>0.3183249829755772</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -5300,8 +5622,8 @@
       <c r="E73" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F73" s="51">
-        <v>0.1680811958081707</v>
+      <c r="F73" s="102">
+        <v>1.267180118981133</v>
       </c>
     </row>
   </sheetData>
@@ -5350,8 +5672,8 @@
       <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="66">
-        <v>2682711.463207951</v>
+      <c r="F2" s="112">
+        <v>2682711.463207952</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -5370,8 +5692,8 @@
       <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="66">
-        <v>2682711.463207951</v>
+      <c r="F3" s="112">
+        <v>2682711.463207952</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -5390,8 +5712,8 @@
       <c r="E4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="66">
-        <v>2682711.463207951</v>
+      <c r="F4" s="112">
+        <v>2682711.463207952</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -5410,8 +5732,8 @@
       <c r="E5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="66">
-        <v>2682711.463207951</v>
+      <c r="F5" s="112">
+        <v>2682711.463207952</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -5430,8 +5752,8 @@
       <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="66">
-        <v>2682711.463207951</v>
+      <c r="F6" s="112">
+        <v>2682711.463207952</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -5450,8 +5772,8 @@
       <c r="E7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="66">
-        <v>2682711.463207951</v>
+      <c r="F7" s="112">
+        <v>2682711.463207952</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -5470,8 +5792,8 @@
       <c r="E8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="66">
-        <v>2682711.463207951</v>
+      <c r="F8" s="112">
+        <v>2682711.463207952</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -5490,8 +5812,8 @@
       <c r="E9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="66">
-        <v>2682711.463207951</v>
+      <c r="F9" s="112">
+        <v>2682711.463207952</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -5510,8 +5832,8 @@
       <c r="E10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="66">
-        <v>2682711.463207951</v>
+      <c r="F10" s="112">
+        <v>2682711.463207952</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -5530,8 +5852,8 @@
       <c r="E11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="66">
-        <v>2682711.463207951</v>
+      <c r="F11" s="112">
+        <v>2682711.463207952</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -5550,8 +5872,8 @@
       <c r="E12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="66">
-        <v>2682711.463207951</v>
+      <c r="F12" s="112">
+        <v>2682711.463207952</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -5570,8 +5892,8 @@
       <c r="E13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="66">
-        <v>2682711.463207951</v>
+      <c r="F13" s="112">
+        <v>2682711.463207952</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -5590,8 +5912,8 @@
       <c r="E14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="66">
-        <v>2682711.463207951</v>
+      <c r="F14" s="112">
+        <v>2682711.463207952</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -5610,8 +5932,8 @@
       <c r="E15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="66">
-        <v>2682711.463207951</v>
+      <c r="F15" s="112">
+        <v>2682711.463207952</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -5630,8 +5952,8 @@
       <c r="E16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="66">
-        <v>2682711.463207951</v>
+      <c r="F16" s="112">
+        <v>2682711.463207952</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -5650,8 +5972,8 @@
       <c r="E17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="66">
-        <v>2682711.463207951</v>
+      <c r="F17" s="112">
+        <v>2682711.463207952</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -5670,8 +5992,8 @@
       <c r="E18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="66">
-        <v>2682711.463207951</v>
+      <c r="F18" s="112">
+        <v>2682711.463207952</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -5690,8 +6012,8 @@
       <c r="E19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="66">
-        <v>2682711.463207951</v>
+      <c r="F19" s="112">
+        <v>2682711.463207952</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -5710,8 +6032,8 @@
       <c r="E20" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F20" s="66">
-        <v>2682711.463207951</v>
+      <c r="F20" s="112">
+        <v>2682711.463207952</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -5730,8 +6052,8 @@
       <c r="E21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F21" s="66">
-        <v>2682711.463207951</v>
+      <c r="F21" s="112">
+        <v>2682711.463207952</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -5750,8 +6072,8 @@
       <c r="E22" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F22" s="66">
-        <v>2682711.463207951</v>
+      <c r="F22" s="112">
+        <v>2682711.463207952</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -5770,8 +6092,8 @@
       <c r="E23" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="66">
-        <v>2682711.463207951</v>
+      <c r="F23" s="112">
+        <v>2682711.463207952</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -5790,8 +6112,8 @@
       <c r="E24" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F24" s="66">
-        <v>2682711.463207951</v>
+      <c r="F24" s="112">
+        <v>2682711.463207952</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -5810,8 +6132,8 @@
       <c r="E25" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F25" s="66">
-        <v>2682711.463207951</v>
+      <c r="F25" s="112">
+        <v>2682711.463207952</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -5830,8 +6152,8 @@
       <c r="E26" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F26" s="66">
-        <v>2682711.463207951</v>
+      <c r="F26" s="112">
+        <v>2682711.463207952</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -5850,8 +6172,8 @@
       <c r="E27" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F27" s="66">
-        <v>2682711.463207951</v>
+      <c r="F27" s="112">
+        <v>2682711.463207952</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -5870,8 +6192,8 @@
       <c r="E28" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F28" s="66">
-        <v>2682711.463207951</v>
+      <c r="F28" s="112">
+        <v>2682711.463207952</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -5890,8 +6212,8 @@
       <c r="E29" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="66">
-        <v>2682711.463207951</v>
+      <c r="F29" s="112">
+        <v>2682711.463207952</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -5910,8 +6232,8 @@
       <c r="E30" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F30" s="66">
-        <v>2682711.463207951</v>
+      <c r="F30" s="112">
+        <v>2682711.463207952</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -5930,8 +6252,8 @@
       <c r="E31" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F31" s="66">
-        <v>2682711.463207951</v>
+      <c r="F31" s="112">
+        <v>2682711.463207952</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -5950,8 +6272,8 @@
       <c r="E32" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F32" s="66">
-        <v>2682711.463207951</v>
+      <c r="F32" s="112">
+        <v>2682711.463207952</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -5970,8 +6292,8 @@
       <c r="E33" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F33" s="66">
-        <v>2682711.463207951</v>
+      <c r="F33" s="112">
+        <v>2682711.463207952</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -5990,8 +6312,8 @@
       <c r="E34" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F34" s="66">
-        <v>2682711.463207951</v>
+      <c r="F34" s="112">
+        <v>2682711.463207952</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -6010,8 +6332,8 @@
       <c r="E35" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F35" s="66">
-        <v>2682711.463207951</v>
+      <c r="F35" s="112">
+        <v>2682711.463207952</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -6030,8 +6352,8 @@
       <c r="E36" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F36" s="66">
-        <v>2682711.463207951</v>
+      <c r="F36" s="112">
+        <v>2682711.463207952</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -6050,8 +6372,8 @@
       <c r="E37" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F37" s="66">
-        <v>2682711.463207951</v>
+      <c r="F37" s="112">
+        <v>2682711.463207952</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -6070,8 +6392,8 @@
       <c r="E38" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F38" s="67">
-        <v>3303079.964256136</v>
+      <c r="F38" s="113">
+        <v>3303079.964256137</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -6090,8 +6412,8 @@
       <c r="E39" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F39" s="67">
-        <v>3303079.964256136</v>
+      <c r="F39" s="113">
+        <v>3303079.964256137</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -6110,8 +6432,8 @@
       <c r="E40" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F40" s="67">
-        <v>3303079.964256136</v>
+      <c r="F40" s="113">
+        <v>3303079.964256137</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -6130,8 +6452,8 @@
       <c r="E41" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F41" s="67">
-        <v>3303079.964256136</v>
+      <c r="F41" s="113">
+        <v>3303079.964256137</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -6150,8 +6472,8 @@
       <c r="E42" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F42" s="67">
-        <v>3303079.964256136</v>
+      <c r="F42" s="113">
+        <v>3303079.964256137</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -6170,8 +6492,8 @@
       <c r="E43" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F43" s="67">
-        <v>3303079.964256136</v>
+      <c r="F43" s="113">
+        <v>3303079.964256137</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -6190,8 +6512,8 @@
       <c r="E44" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F44" s="67">
-        <v>3303079.964256136</v>
+      <c r="F44" s="113">
+        <v>3303079.964256137</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -6210,8 +6532,8 @@
       <c r="E45" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F45" s="67">
-        <v>3303079.964256136</v>
+      <c r="F45" s="113">
+        <v>3303079.964256137</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -6230,8 +6552,8 @@
       <c r="E46" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F46" s="67">
-        <v>3303079.964256136</v>
+      <c r="F46" s="113">
+        <v>3303079.964256137</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -6250,8 +6572,8 @@
       <c r="E47" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F47" s="67">
-        <v>3303079.964256136</v>
+      <c r="F47" s="113">
+        <v>3303079.964256137</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -6270,8 +6592,8 @@
       <c r="E48" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F48" s="67">
-        <v>3303079.964256136</v>
+      <c r="F48" s="113">
+        <v>3303079.964256137</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -6290,8 +6612,8 @@
       <c r="E49" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F49" s="67">
-        <v>3303079.964256136</v>
+      <c r="F49" s="113">
+        <v>3303079.964256137</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -6310,8 +6632,8 @@
       <c r="E50" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F50" s="67">
-        <v>3303079.964256136</v>
+      <c r="F50" s="113">
+        <v>3303079.964256137</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -6330,8 +6652,8 @@
       <c r="E51" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F51" s="67">
-        <v>3303079.964256136</v>
+      <c r="F51" s="113">
+        <v>3303079.964256137</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -6350,8 +6672,8 @@
       <c r="E52" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F52" s="67">
-        <v>3303079.964256136</v>
+      <c r="F52" s="113">
+        <v>3303079.964256137</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -6370,8 +6692,8 @@
       <c r="E53" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F53" s="67">
-        <v>3303079.964256136</v>
+      <c r="F53" s="113">
+        <v>3303079.964256137</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -6390,8 +6712,8 @@
       <c r="E54" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F54" s="67">
-        <v>3303079.964256136</v>
+      <c r="F54" s="113">
+        <v>3303079.964256137</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -6410,8 +6732,8 @@
       <c r="E55" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F55" s="67">
-        <v>3303079.964256136</v>
+      <c r="F55" s="113">
+        <v>3303079.964256137</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -6430,8 +6752,8 @@
       <c r="E56" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F56" s="67">
-        <v>3303079.964256136</v>
+      <c r="F56" s="113">
+        <v>3303079.964256137</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -6450,8 +6772,8 @@
       <c r="E57" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F57" s="67">
-        <v>3303079.964256136</v>
+      <c r="F57" s="113">
+        <v>3303079.964256137</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -6470,8 +6792,8 @@
       <c r="E58" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F58" s="67">
-        <v>3303079.964256136</v>
+      <c r="F58" s="113">
+        <v>3303079.964256137</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -6490,8 +6812,8 @@
       <c r="E59" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F59" s="67">
-        <v>3303079.964256136</v>
+      <c r="F59" s="113">
+        <v>3303079.964256137</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -6510,8 +6832,8 @@
       <c r="E60" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F60" s="67">
-        <v>3303079.964256136</v>
+      <c r="F60" s="113">
+        <v>3303079.964256137</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -6530,8 +6852,8 @@
       <c r="E61" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F61" s="67">
-        <v>3303079.964256136</v>
+      <c r="F61" s="113">
+        <v>3303079.964256137</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -6550,8 +6872,8 @@
       <c r="E62" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F62" s="67">
-        <v>3303079.964256136</v>
+      <c r="F62" s="113">
+        <v>3303079.964256137</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -6570,8 +6892,8 @@
       <c r="E63" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F63" s="67">
-        <v>3303079.964256136</v>
+      <c r="F63" s="113">
+        <v>3303079.964256137</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -6590,8 +6912,8 @@
       <c r="E64" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F64" s="67">
-        <v>3303079.964256136</v>
+      <c r="F64" s="113">
+        <v>3303079.964256137</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -6610,8 +6932,8 @@
       <c r="E65" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F65" s="67">
-        <v>3303079.964256136</v>
+      <c r="F65" s="113">
+        <v>3303079.964256137</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -6630,8 +6952,8 @@
       <c r="E66" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F66" s="67">
-        <v>3303079.964256136</v>
+      <c r="F66" s="113">
+        <v>3303079.964256137</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -6650,8 +6972,8 @@
       <c r="E67" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F67" s="67">
-        <v>3303079.964256136</v>
+      <c r="F67" s="113">
+        <v>3303079.964256137</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -6670,8 +6992,8 @@
       <c r="E68" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F68" s="67">
-        <v>3303079.964256136</v>
+      <c r="F68" s="113">
+        <v>3303079.964256137</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -6690,8 +7012,8 @@
       <c r="E69" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F69" s="67">
-        <v>3303079.964256136</v>
+      <c r="F69" s="113">
+        <v>3303079.964256137</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -6710,8 +7032,8 @@
       <c r="E70" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F70" s="67">
-        <v>3303079.964256136</v>
+      <c r="F70" s="113">
+        <v>3303079.964256137</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -6730,8 +7052,8 @@
       <c r="E71" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F71" s="67">
-        <v>3303079.964256136</v>
+      <c r="F71" s="113">
+        <v>3303079.964256137</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -6750,8 +7072,8 @@
       <c r="E72" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F72" s="67">
-        <v>3303079.964256136</v>
+      <c r="F72" s="113">
+        <v>3303079.964256137</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -6770,8 +7092,8 @@
       <c r="E73" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F73" s="67">
-        <v>3303079.964256136</v>
+      <c r="F73" s="113">
+        <v>3303079.964256137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created shares installed figure and updated multi
</commit_message>
<xml_diff>
--- a/results/Manuscript/total_capacity.xlsx
+++ b/results/Manuscript/total_capacity.xlsx
@@ -820,8 +820,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -829,8 +829,8 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -838,27 +838,27 @@
     <xf numFmtId="0" fontId="3" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -872,8 +872,8 @@
     <xf numFmtId="0" fontId="2" fillId="53" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="54" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="55" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="56" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="57" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="56" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="57" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="58" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="59" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="60" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -881,12 +881,12 @@
     <xf numFmtId="0" fontId="2" fillId="62" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="63" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="64" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="65" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="65" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="66" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="67" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="68" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="69" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="70" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="70" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="71" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="72" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="73" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1323,7 +1323,7 @@
         <v>11</v>
       </c>
       <c r="F5" s="4">
-        <v>483.12078453503</v>
+        <v>483.1207845350301</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1343,7 +1343,7 @@
         <v>14</v>
       </c>
       <c r="F6" s="5">
-        <v>923.1831725841055</v>
+        <v>923.1831725841057</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1363,7 +1363,7 @@
         <v>15</v>
       </c>
       <c r="F7" s="6">
-        <v>1152.751003947368</v>
+        <v>1152.751003947369</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1583,7 +1583,7 @@
         <v>14</v>
       </c>
       <c r="F18" s="14">
-        <v>977.8659786286419</v>
+        <v>977.8659786286421</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1623,7 +1623,7 @@
         <v>11</v>
       </c>
       <c r="F20" s="16">
-        <v>627.2015891316861</v>
+        <v>627.2015891316862</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1863,7 +1863,7 @@
         <v>11</v>
       </c>
       <c r="F32" s="24">
-        <v>644.9321684842531</v>
+        <v>644.9321684842532</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1903,7 +1903,7 @@
         <v>15</v>
       </c>
       <c r="F34" s="26">
-        <v>2027.849145965239</v>
+        <v>2027.849145965238</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1923,7 +1923,7 @@
         <v>11</v>
       </c>
       <c r="F35" s="27">
-        <v>639.4866324486115</v>
+        <v>639.4866324486113</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1963,7 +1963,7 @@
         <v>15</v>
       </c>
       <c r="F37" s="26">
-        <v>2029.720920787313</v>
+        <v>2029.720920787312</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -2063,7 +2063,7 @@
         <v>14</v>
       </c>
       <c r="F42" s="30">
-        <v>1117.765513126117</v>
+        <v>1117.765513126118</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -2103,7 +2103,7 @@
         <v>11</v>
       </c>
       <c r="F44" s="27">
-        <v>641.1266007144516</v>
+        <v>641.1266007144515</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -2123,7 +2123,7 @@
         <v>14</v>
       </c>
       <c r="F45" s="32">
-        <v>1480.185886249178</v>
+        <v>1480.185886249179</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -2163,7 +2163,7 @@
         <v>11</v>
       </c>
       <c r="F47" s="27">
-        <v>637.9581645781425</v>
+        <v>637.9581645781423</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -2283,7 +2283,7 @@
         <v>11</v>
       </c>
       <c r="F53" s="10">
-        <v>578.6995966935914</v>
+        <v>578.699596693591</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -2363,7 +2363,7 @@
         <v>14</v>
       </c>
       <c r="F57" s="39">
-        <v>1499.453134140224</v>
+        <v>1499.453134140225</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -2403,7 +2403,7 @@
         <v>11</v>
       </c>
       <c r="F59" s="38">
-        <v>651.7108701284687</v>
+        <v>651.7108701284689</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -2443,7 +2443,7 @@
         <v>15</v>
       </c>
       <c r="F61" s="41">
-        <v>2057.710104037031</v>
+        <v>2057.71010403703</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -2523,7 +2523,7 @@
         <v>11</v>
       </c>
       <c r="F65" s="42">
-        <v>619.8700563430664</v>
+        <v>619.8700563430662</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -2543,7 +2543,7 @@
         <v>14</v>
       </c>
       <c r="F66" s="43">
-        <v>1263.869862652072</v>
+        <v>1263.869862652073</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -2583,7 +2583,7 @@
         <v>11</v>
       </c>
       <c r="F68" s="38">
-        <v>659.0796714290118</v>
+        <v>659.0796714290116</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -2643,7 +2643,7 @@
         <v>11</v>
       </c>
       <c r="F71" s="38">
-        <v>657.2982506168862</v>
+        <v>657.298250616886</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -2973,7 +2973,7 @@
         <v>11</v>
       </c>
       <c r="F14" s="48">
-        <v>616.2619429148439</v>
+        <v>616.2619429148438</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2993,7 +2993,7 @@
         <v>14</v>
       </c>
       <c r="F15" s="49">
-        <v>1075.808909626445</v>
+        <v>1075.808909626444</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -3013,7 +3013,7 @@
         <v>15</v>
       </c>
       <c r="F16" s="50">
-        <v>1319.070738412529</v>
+        <v>1319.070738412528</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -3033,7 +3033,7 @@
         <v>11</v>
       </c>
       <c r="F17" s="51">
-        <v>68.62344430462659</v>
+        <v>68.62344430462662</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -3073,7 +3073,7 @@
         <v>15</v>
       </c>
       <c r="F19" s="53">
-        <v>364.4666266399108</v>
+        <v>364.4666266399109</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -3113,7 +3113,7 @@
         <v>14</v>
       </c>
       <c r="F21" s="51">
-        <v>60.37855996830722</v>
+        <v>60.37855996830721</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -3133,7 +3133,7 @@
         <v>15</v>
       </c>
       <c r="F22" s="55">
-        <v>53.87988420038165</v>
+        <v>53.87988420038161</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -3153,7 +3153,7 @@
         <v>11</v>
       </c>
       <c r="F23" s="54">
-        <v>33.12524638344903</v>
+        <v>33.12524638344904</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -3173,7 +3173,7 @@
         <v>14</v>
       </c>
       <c r="F24" s="55">
-        <v>53.49084226871565</v>
+        <v>53.49084226871564</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -3193,7 +3193,7 @@
         <v>15</v>
       </c>
       <c r="F25" s="55">
-        <v>50.99647979473985</v>
+        <v>50.99647979473984</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -3333,7 +3333,7 @@
         <v>11</v>
       </c>
       <c r="F32" s="51">
-        <v>58.28292627013489</v>
+        <v>58.2829262701349</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -3373,7 +3373,7 @@
         <v>15</v>
       </c>
       <c r="F34" s="62">
-        <v>173.1823420834153</v>
+        <v>173.1823420834154</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -3393,7 +3393,7 @@
         <v>11</v>
       </c>
       <c r="F35" s="63">
-        <v>70.56254658121432</v>
+        <v>70.56254658121431</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -3433,7 +3433,7 @@
         <v>15</v>
       </c>
       <c r="F37" s="62">
-        <v>168.6425823170192</v>
+        <v>168.6425823170193</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -3693,7 +3693,7 @@
         <v>11</v>
       </c>
       <c r="F50" s="64">
-        <v>759.2297272366443</v>
+        <v>759.2297272366442</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -3833,7 +3833,7 @@
         <v>14</v>
       </c>
       <c r="F57" s="54">
-        <v>27.72313477612434</v>
+        <v>27.72313477612435</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -3853,7 +3853,7 @@
         <v>15</v>
       </c>
       <c r="F58" s="69">
-        <v>20.24594606881279</v>
+        <v>20.24594606881278</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -3873,7 +3873,7 @@
         <v>11</v>
       </c>
       <c r="F59" s="69">
-        <v>19.23173885121909</v>
+        <v>19.2317388512191</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -4033,7 +4033,7 @@
         <v>15</v>
       </c>
       <c r="F67" s="74">
-        <v>1276.88334455429</v>
+        <v>1276.883344554291</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -4053,7 +4053,7 @@
         <v>11</v>
       </c>
       <c r="F68" s="69">
-        <v>25.55812244389284</v>
+        <v>25.55812244389283</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -4073,7 +4073,7 @@
         <v>14</v>
       </c>
       <c r="F69" s="75">
-        <v>85.04682687406506</v>
+        <v>85.04682687406503</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -4113,7 +4113,7 @@
         <v>11</v>
       </c>
       <c r="F71" s="54">
-        <v>29.69897916076388</v>
+        <v>29.69897916076389</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -4133,7 +4133,7 @@
         <v>14</v>
       </c>
       <c r="F72" s="76">
-        <v>106.2937780279886</v>
+        <v>106.2937780279885</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -4283,7 +4283,7 @@
         <v>14</v>
       </c>
       <c r="F6" s="81">
-        <v>454.3618084992925</v>
+        <v>454.3618084992924</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -4503,7 +4503,7 @@
         <v>11</v>
       </c>
       <c r="F17" s="91">
-        <v>84.82386276273837</v>
+        <v>84.82386276273839</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -4643,7 +4643,7 @@
         <v>14</v>
       </c>
       <c r="F24" s="97">
-        <v>153.4042032650071</v>
+        <v>153.4042032650072</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -4703,7 +4703,7 @@
         <v>14</v>
       </c>
       <c r="F27" s="100">
-        <v>287.2318664885297</v>
+        <v>287.2318664885298</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -4723,7 +4723,7 @@
         <v>15</v>
       </c>
       <c r="F28" s="101">
-        <v>328.3449640089808</v>
+        <v>328.3449640089807</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -4743,7 +4743,7 @@
         <v>11</v>
       </c>
       <c r="F29" s="102">
-        <v>2.324118779117084</v>
+        <v>2.32411877911707</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -4823,7 +4823,7 @@
         <v>14</v>
       </c>
       <c r="F33" s="104">
-        <v>36.96416854849968</v>
+        <v>36.96416854849969</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -4883,7 +4883,7 @@
         <v>14</v>
       </c>
       <c r="F36" s="86">
-        <v>51.42141036601843</v>
+        <v>51.42141036601842</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -5023,7 +5023,7 @@
         <v>15</v>
       </c>
       <c r="F43" s="107">
-        <v>536.1615916173696</v>
+        <v>536.1615916173694</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -5043,7 +5043,7 @@
         <v>11</v>
       </c>
       <c r="F44" s="94">
-        <v>21.14379388521164</v>
+        <v>21.14379388521163</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -5143,7 +5143,7 @@
         <v>15</v>
       </c>
       <c r="F49" s="86">
-        <v>52.81883861675564</v>
+        <v>52.81883861675566</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -5163,7 +5163,7 @@
         <v>11</v>
       </c>
       <c r="F50" s="108">
-        <v>130.5635813865583</v>
+        <v>130.5635813865584</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -5203,7 +5203,7 @@
         <v>15</v>
       </c>
       <c r="F52" s="109">
-        <v>583.2422931874851</v>
+        <v>583.2422931874853</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -5303,7 +5303,7 @@
         <v>14</v>
       </c>
       <c r="F57" s="111">
-        <v>42.51319236584933</v>
+        <v>42.51319236584932</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -5323,7 +5323,7 @@
         <v>15</v>
       </c>
       <c r="F58" s="96">
-        <v>26.73443233736913</v>
+        <v>26.73443233736914</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -5343,7 +5343,7 @@
         <v>11</v>
       </c>
       <c r="F59" s="99">
-        <v>6.903209387678077</v>
+        <v>6.903209387678072</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -5363,7 +5363,7 @@
         <v>14</v>
       </c>
       <c r="F60" s="86">
-        <v>54.97147660664991</v>
+        <v>54.9714766066499</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -5383,7 +5383,7 @@
         <v>15</v>
       </c>
       <c r="F61" s="96">
-        <v>29.86728322668818</v>
+        <v>29.86728322668819</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -5443,7 +5443,7 @@
         <v>15</v>
       </c>
       <c r="F64" s="86">
-        <v>51.35203405575305</v>
+        <v>51.35203405575294</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -5483,7 +5483,7 @@
         <v>14</v>
       </c>
       <c r="F66" s="86">
-        <v>52.2063639349315</v>
+        <v>52.20636393493147</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -5503,7 +5503,7 @@
         <v>15</v>
       </c>
       <c r="F67" s="99">
-        <v>8.545459160627047</v>
+        <v>8.545459160627033</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -5673,7 +5673,7 @@
         <v>11</v>
       </c>
       <c r="F2" s="112">
-        <v>2682711.463207952</v>
+        <v>2682711.463207951</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -5693,7 +5693,7 @@
         <v>14</v>
       </c>
       <c r="F3" s="112">
-        <v>2682711.463207952</v>
+        <v>2682711.463207951</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -5713,7 +5713,7 @@
         <v>15</v>
       </c>
       <c r="F4" s="112">
-        <v>2682711.463207952</v>
+        <v>2682711.463207951</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -5733,7 +5733,7 @@
         <v>11</v>
       </c>
       <c r="F5" s="112">
-        <v>2682711.463207952</v>
+        <v>2682711.463207951</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -5753,7 +5753,7 @@
         <v>14</v>
       </c>
       <c r="F6" s="112">
-        <v>2682711.463207952</v>
+        <v>2682711.463207951</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -5773,7 +5773,7 @@
         <v>15</v>
       </c>
       <c r="F7" s="112">
-        <v>2682711.463207952</v>
+        <v>2682711.463207951</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -5793,7 +5793,7 @@
         <v>11</v>
       </c>
       <c r="F8" s="112">
-        <v>2682711.463207952</v>
+        <v>2682711.463207951</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -5813,7 +5813,7 @@
         <v>14</v>
       </c>
       <c r="F9" s="112">
-        <v>2682711.463207952</v>
+        <v>2682711.463207951</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -5833,7 +5833,7 @@
         <v>15</v>
       </c>
       <c r="F10" s="112">
-        <v>2682711.463207952</v>
+        <v>2682711.463207951</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -5853,7 +5853,7 @@
         <v>11</v>
       </c>
       <c r="F11" s="112">
-        <v>2682711.463207952</v>
+        <v>2682711.463207951</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -5873,7 +5873,7 @@
         <v>14</v>
       </c>
       <c r="F12" s="112">
-        <v>2682711.463207952</v>
+        <v>2682711.463207951</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -5893,7 +5893,7 @@
         <v>15</v>
       </c>
       <c r="F13" s="112">
-        <v>2682711.463207952</v>
+        <v>2682711.463207951</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -5913,7 +5913,7 @@
         <v>11</v>
       </c>
       <c r="F14" s="112">
-        <v>2682711.463207952</v>
+        <v>2682711.463207951</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -5933,7 +5933,7 @@
         <v>14</v>
       </c>
       <c r="F15" s="112">
-        <v>2682711.463207952</v>
+        <v>2682711.463207951</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -5953,7 +5953,7 @@
         <v>15</v>
       </c>
       <c r="F16" s="112">
-        <v>2682711.463207952</v>
+        <v>2682711.463207951</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -5973,7 +5973,7 @@
         <v>11</v>
       </c>
       <c r="F17" s="112">
-        <v>2682711.463207952</v>
+        <v>2682711.463207951</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -5993,7 +5993,7 @@
         <v>14</v>
       </c>
       <c r="F18" s="112">
-        <v>2682711.463207952</v>
+        <v>2682711.463207951</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -6013,7 +6013,7 @@
         <v>15</v>
       </c>
       <c r="F19" s="112">
-        <v>2682711.463207952</v>
+        <v>2682711.463207951</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -6033,7 +6033,7 @@
         <v>11</v>
       </c>
       <c r="F20" s="112">
-        <v>2682711.463207952</v>
+        <v>2682711.463207951</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -6053,7 +6053,7 @@
         <v>14</v>
       </c>
       <c r="F21" s="112">
-        <v>2682711.463207952</v>
+        <v>2682711.463207951</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -6073,7 +6073,7 @@
         <v>15</v>
       </c>
       <c r="F22" s="112">
-        <v>2682711.463207952</v>
+        <v>2682711.463207951</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -6093,7 +6093,7 @@
         <v>11</v>
       </c>
       <c r="F23" s="112">
-        <v>2682711.463207952</v>
+        <v>2682711.463207951</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -6113,7 +6113,7 @@
         <v>14</v>
       </c>
       <c r="F24" s="112">
-        <v>2682711.463207952</v>
+        <v>2682711.463207951</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -6133,7 +6133,7 @@
         <v>15</v>
       </c>
       <c r="F25" s="112">
-        <v>2682711.463207952</v>
+        <v>2682711.463207951</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -6153,7 +6153,7 @@
         <v>11</v>
       </c>
       <c r="F26" s="112">
-        <v>2682711.463207952</v>
+        <v>2682711.463207951</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -6173,7 +6173,7 @@
         <v>14</v>
       </c>
       <c r="F27" s="112">
-        <v>2682711.463207952</v>
+        <v>2682711.463207951</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -6193,7 +6193,7 @@
         <v>15</v>
       </c>
       <c r="F28" s="112">
-        <v>2682711.463207952</v>
+        <v>2682711.463207951</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -6213,7 +6213,7 @@
         <v>11</v>
       </c>
       <c r="F29" s="112">
-        <v>2682711.463207952</v>
+        <v>2682711.463207951</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -6233,7 +6233,7 @@
         <v>14</v>
       </c>
       <c r="F30" s="112">
-        <v>2682711.463207952</v>
+        <v>2682711.463207951</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -6253,7 +6253,7 @@
         <v>15</v>
       </c>
       <c r="F31" s="112">
-        <v>2682711.463207952</v>
+        <v>2682711.463207951</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -6273,7 +6273,7 @@
         <v>11</v>
       </c>
       <c r="F32" s="112">
-        <v>2682711.463207952</v>
+        <v>2682711.463207951</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -6293,7 +6293,7 @@
         <v>14</v>
       </c>
       <c r="F33" s="112">
-        <v>2682711.463207952</v>
+        <v>2682711.463207951</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -6313,7 +6313,7 @@
         <v>15</v>
       </c>
       <c r="F34" s="112">
-        <v>2682711.463207952</v>
+        <v>2682711.463207951</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -6333,7 +6333,7 @@
         <v>11</v>
       </c>
       <c r="F35" s="112">
-        <v>2682711.463207952</v>
+        <v>2682711.463207951</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -6353,7 +6353,7 @@
         <v>14</v>
       </c>
       <c r="F36" s="112">
-        <v>2682711.463207952</v>
+        <v>2682711.463207951</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -6373,7 +6373,7 @@
         <v>15</v>
       </c>
       <c r="F37" s="112">
-        <v>2682711.463207952</v>
+        <v>2682711.463207951</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -6393,7 +6393,7 @@
         <v>11</v>
       </c>
       <c r="F38" s="113">
-        <v>3303079.964256137</v>
+        <v>3303079.964256136</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -6413,7 +6413,7 @@
         <v>14</v>
       </c>
       <c r="F39" s="113">
-        <v>3303079.964256137</v>
+        <v>3303079.964256136</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -6433,7 +6433,7 @@
         <v>15</v>
       </c>
       <c r="F40" s="113">
-        <v>3303079.964256137</v>
+        <v>3303079.964256136</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -6453,7 +6453,7 @@
         <v>11</v>
       </c>
       <c r="F41" s="113">
-        <v>3303079.964256137</v>
+        <v>3303079.964256136</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -6473,7 +6473,7 @@
         <v>14</v>
       </c>
       <c r="F42" s="113">
-        <v>3303079.964256137</v>
+        <v>3303079.964256136</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -6493,7 +6493,7 @@
         <v>15</v>
       </c>
       <c r="F43" s="113">
-        <v>3303079.964256137</v>
+        <v>3303079.964256136</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -6513,7 +6513,7 @@
         <v>11</v>
       </c>
       <c r="F44" s="113">
-        <v>3303079.964256137</v>
+        <v>3303079.964256136</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -6533,7 +6533,7 @@
         <v>14</v>
       </c>
       <c r="F45" s="113">
-        <v>3303079.964256137</v>
+        <v>3303079.964256136</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -6553,7 +6553,7 @@
         <v>15</v>
       </c>
       <c r="F46" s="113">
-        <v>3303079.964256137</v>
+        <v>3303079.964256136</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -6573,7 +6573,7 @@
         <v>11</v>
       </c>
       <c r="F47" s="113">
-        <v>3303079.964256137</v>
+        <v>3303079.964256136</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -6593,7 +6593,7 @@
         <v>14</v>
       </c>
       <c r="F48" s="113">
-        <v>3303079.964256137</v>
+        <v>3303079.964256136</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -6613,7 +6613,7 @@
         <v>15</v>
       </c>
       <c r="F49" s="113">
-        <v>3303079.964256137</v>
+        <v>3303079.964256136</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -6633,7 +6633,7 @@
         <v>11</v>
       </c>
       <c r="F50" s="113">
-        <v>3303079.964256137</v>
+        <v>3303079.964256136</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -6653,7 +6653,7 @@
         <v>14</v>
       </c>
       <c r="F51" s="113">
-        <v>3303079.964256137</v>
+        <v>3303079.964256136</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -6673,7 +6673,7 @@
         <v>15</v>
       </c>
       <c r="F52" s="113">
-        <v>3303079.964256137</v>
+        <v>3303079.964256136</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -6693,7 +6693,7 @@
         <v>11</v>
       </c>
       <c r="F53" s="113">
-        <v>3303079.964256137</v>
+        <v>3303079.964256136</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -6713,7 +6713,7 @@
         <v>14</v>
       </c>
       <c r="F54" s="113">
-        <v>3303079.964256137</v>
+        <v>3303079.964256136</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -6733,7 +6733,7 @@
         <v>15</v>
       </c>
       <c r="F55" s="113">
-        <v>3303079.964256137</v>
+        <v>3303079.964256136</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -6753,7 +6753,7 @@
         <v>11</v>
       </c>
       <c r="F56" s="113">
-        <v>3303079.964256137</v>
+        <v>3303079.964256136</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -6773,7 +6773,7 @@
         <v>14</v>
       </c>
       <c r="F57" s="113">
-        <v>3303079.964256137</v>
+        <v>3303079.964256136</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -6793,7 +6793,7 @@
         <v>15</v>
       </c>
       <c r="F58" s="113">
-        <v>3303079.964256137</v>
+        <v>3303079.964256136</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -6813,7 +6813,7 @@
         <v>11</v>
       </c>
       <c r="F59" s="113">
-        <v>3303079.964256137</v>
+        <v>3303079.964256136</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -6833,7 +6833,7 @@
         <v>14</v>
       </c>
       <c r="F60" s="113">
-        <v>3303079.964256137</v>
+        <v>3303079.964256136</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -6853,7 +6853,7 @@
         <v>15</v>
       </c>
       <c r="F61" s="113">
-        <v>3303079.964256137</v>
+        <v>3303079.964256136</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -6873,7 +6873,7 @@
         <v>11</v>
       </c>
       <c r="F62" s="113">
-        <v>3303079.964256137</v>
+        <v>3303079.964256136</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -6893,7 +6893,7 @@
         <v>14</v>
       </c>
       <c r="F63" s="113">
-        <v>3303079.964256137</v>
+        <v>3303079.964256136</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -6913,7 +6913,7 @@
         <v>15</v>
       </c>
       <c r="F64" s="113">
-        <v>3303079.964256137</v>
+        <v>3303079.964256136</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -6933,7 +6933,7 @@
         <v>11</v>
       </c>
       <c r="F65" s="113">
-        <v>3303079.964256137</v>
+        <v>3303079.964256136</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -6953,7 +6953,7 @@
         <v>14</v>
       </c>
       <c r="F66" s="113">
-        <v>3303079.964256137</v>
+        <v>3303079.964256136</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -6973,7 +6973,7 @@
         <v>15</v>
       </c>
       <c r="F67" s="113">
-        <v>3303079.964256137</v>
+        <v>3303079.964256136</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -6993,7 +6993,7 @@
         <v>11</v>
       </c>
       <c r="F68" s="113">
-        <v>3303079.964256137</v>
+        <v>3303079.964256136</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -7013,7 +7013,7 @@
         <v>14</v>
       </c>
       <c r="F69" s="113">
-        <v>3303079.964256137</v>
+        <v>3303079.964256136</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -7033,7 +7033,7 @@
         <v>15</v>
       </c>
       <c r="F70" s="113">
-        <v>3303079.964256137</v>
+        <v>3303079.964256136</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -7053,7 +7053,7 @@
         <v>11</v>
       </c>
       <c r="F71" s="113">
-        <v>3303079.964256137</v>
+        <v>3303079.964256136</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -7073,7 +7073,7 @@
         <v>14</v>
       </c>
       <c r="F72" s="113">
-        <v>3303079.964256137</v>
+        <v>3303079.964256136</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -7093,7 +7093,7 @@
         <v>15</v>
       </c>
       <c r="F73" s="113">
-        <v>3303079.964256137</v>
+        <v>3303079.964256136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>